<commit_message>
Adicionando  a planilha de testes
</commit_message>
<xml_diff>
--- a/dados/Valorant.xlsx
+++ b/dados/Valorant.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabri\OneDrive\Area_de _trabalho\Cdados\Projeto 1\Projeto1-Cdados\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E1ABFE-4993-43EF-A3B7-094E9D76D107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE78CD62-68FD-433E-8919-25A3013F1A99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
-    <sheet name="Teste" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="501">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1818,192 +1817,6 @@
   </si>
   <si>
     <t>quem vai jogar um valorant cmg hj</t>
-  </si>
-  <si>
-    <t>Teste</t>
-  </si>
-  <si>
-    <t>mt silverio abandona a carreira como dj e vira pro player de valorant, em breve nos cinemas</t>
-  </si>
-  <si>
-    <t>definitivamente o valorant n quer mais me ver jogar, é cada bronze com jogatina de imortal q pelamor</t>
-  </si>
-  <si>
-    <t>eu jogando valorant com meus amigos // eu jogando valorant sozinho https://t.co/esjhdslejb</t>
-  </si>
-  <si>
-    <t>eu sei que a minha equipa no valorant é má quando sou eu a top fragger</t>
-  </si>
-  <si>
-    <t>baixei valorant.. esse foi o erro da noite kkk</t>
-  </si>
-  <si>
-    <t>rt @godz3r4: era só um valorant com a dudik pra por um sorriso no meu rosto</t>
-  </si>
-  <si>
-    <t>fodase agora eu sou pro player de lol e de valorant</t>
-  </si>
-  <si>
-    <t>eu n ganhei u m a partida hohe no valorant uma uma uma n ganhei umaaaaaa</t>
-  </si>
-  <si>
-    <t>rt @hellzfps: as skins spline do valorant parecem aquele arame de amarrar embalagem de pão fatiado e eu posso provar https://t.co/xfdusm9qvt</t>
-  </si>
-  <si>
-    <t>minha muie aprendendo a joga valorant as 3 da manha enquanto eu morro de rinite no fundo https://t.co/vukpcq6msj</t>
-  </si>
-  <si>
-    <t>bom dia, hoje eu hard vou produzir um conteúdo diferenciado, o que acontece quando você joga bêbado valorant .
-querem saber mais ? esperem mais tarde 😁</t>
-  </si>
-  <si>
-    <t>abre o valorant pra se divertir um tico depois dum dia cansativo &amp;gt; cai na partida com um cara abre o microfone pra arrotar</t>
-  </si>
-  <si>
-    <t>desgraça só pego gente enviada pelo maligno pra jogar cmg n valorant pq pqp não tem como ser tão horríveis vai tomar no cu</t>
-  </si>
-  <si>
-    <t>valorant o jogo do amor</t>
-  </si>
-  <si>
-    <t>finalmente vou conseguir valorant🙏🙏
-finalmente os mimos🙏</t>
-  </si>
-  <si>
-    <t>tô curtindo o valorant! :)</t>
-  </si>
-  <si>
-    <t>rt @relatosfrases: quem joga valorant? bora jogar uma agora?</t>
-  </si>
-  <si>
-    <t>coisas bullet sobre mim
-altura- 1,92
-numero do calçado- 43
-signo/mbti- peixes/???
-tattoo - 0
-piercings- 0
-cor - verde
-série fav - vikings 
-anime fav- ?
-comida - tanto faz 
-bebida- sei lá 
-jogo fav- valorant https://t.co/5b3d2y3xdn</t>
-  </si>
-  <si>
-    <t>valorant me deixa tão feliz e irritado ao mesmo tempo pqp</t>
-  </si>
-  <si>
-    <t>rt @sofiaespanha: caralho cai contra um time com 3 racistas no valorant hoje, cada dia a comunidade ta mais tóxica</t>
-  </si>
-  <si>
-    <t>@rhalekey bora, mas agr no, to jogando valorant</t>
-  </si>
-  <si>
-    <t>acabei de gastar 120 reais pra pegar uma faquinha no valorant 🤡🤡🤡🤡🤡🤡🤡🤡🤡🤡🤡</t>
-  </si>
-  <si>
-    <t>altura— 1,62
-idade— 21
-tamanho do pé— 37
-signo— escorpiao
-tatuagens— 0
-piercing— 0
-cor fav— rosa branco e preto q nem avril lavigne em 2007
-série fav— no momento hello my twenties
-animal fav— cachorro
-comida favー feijoada
-bebida fav— suco de laranja c morango
-jogo fav— valorant https://t.co/fpvo7z2zzr</t>
-  </si>
-  <si>
-    <t>rt @phzkkj: parabéns velho você é o cara mais foda que existe você é bom em tudo, valorant design e arte digital o vic é o mais brabo https…</t>
-  </si>
-  <si>
-    <t>@patrurr @maxgpi_ prende valorant patra lul</t>
-  </si>
-  <si>
-    <t>@blxckoutz skill base do valorant é uma merda, ate parece que o venoninho realmente tem nível pra ta ai, server br que fala</t>
-  </si>
-  <si>
-    <t>rt @garamops: tá chegando o dia!!! os dois primeiros colocados garantem vaga no major league de valorant, realizado pela @sourivals.
-🗓 16/…</t>
-  </si>
-  <si>
-    <t>@tigreanao @victorra33 @xzerthe @lucassi87814842 @valorantbrasil e de teclado e mouse
-vai ser muito roubado ent n tem como o valorant ir pra console</t>
-  </si>
-  <si>
-    <t>alguém p jogar valorant comigo agoraaaaa???</t>
-  </si>
-  <si>
-    <t>irmão eu não consigo acabar o passe do valorant pqp</t>
-  </si>
-  <si>
-    <t>eu só queria tá jogando um valorant com os cria agr</t>
-  </si>
-  <si>
-    <t>rt @dwkndhxt: kkkkkkkkkl realmente #valorant https://t.co/tgohv3pyy8</t>
-  </si>
-  <si>
-    <t>primeiro vídeo no canal! https://t.co/szejulvouc #valorant #colombera182 #colomverso #twitch #twitchstreamer #twitchaffiliate</t>
-  </si>
-  <si>
-    <t>@sciponnk no valorant eu era horrível mas eu tinha time pq meus amigos eram paneleiros, agr no fort o pai #deita</t>
-  </si>
-  <si>
-    <t>miau caralho #valorant
-🔗 https://t.co/04c8vbndom https://t.co/bot6xfka1k</t>
-  </si>
-  <si>
-    <t>jogando com promesas do xile na valorant https://t.co/rzokpbpadn</t>
-  </si>
-  <si>
-    <t>@xavicalo boa noite xavica, como vai? farmando muito o passe do valorant?</t>
-  </si>
-  <si>
-    <t>@miggsmootinha naum o do valorant</t>
-  </si>
-  <si>
-    <t>uma curtida e eu vou joga valorant...</t>
-  </si>
-  <si>
-    <t>velho, a killjoy tem a dublagem mais genial do valorant e ngm tira isso da minha cabeça, pqp kkkkkkkk
-todos tiram sarro da efixiência alemã, ho-hoh… isso, ri mexmo, enquanto usa as coisax q eu criei…
-e eu fzr cover das falas ao vivo pqp ksksksksksk</t>
-  </si>
-  <si>
-    <t>coisas inúteis sobre mim... 
-altura - 1.61
-numero do calçado - 38
-signo/mbti - leão/infj
-tattoo - 0
-piercings - 0
-cor - rosa
-série fav - x files
-anime fav - kobato
-comida - sushi
-bebida - agua de côco 
-jogo fav - valorant
-boring https://t.co/65t1lv0mpf</t>
-  </si>
-  <si>
-    <t>tamos ai a mandar 4k's como se nao houvesse amanha
-@valorant_pt https://t.co/fcehymp7ju</t>
-  </si>
-  <si>
-    <t>jogo desgraçado esse valorant toma no cu</t>
-  </si>
-  <si>
-    <t>mentira vou continuar jogando valorant msm fds</t>
-  </si>
-  <si>
-    <t>to me sentindo sozinha vo joga valorant</t>
-  </si>
-  <si>
-    <t>@mavironas @tmrzin @drxkonz @tisxra mds mano qq se ta falando ele nem ta faland por ele, ele so ta farpando o its felipe que ele falou pro tisoura ir pro valorant ai o dk so tava zuando o sequela</t>
-  </si>
-  <si>
-    <t>@tisxra feliz aniversario agora tu pode competir no valorant 👍</t>
   </si>
 </sst>
 </file>
@@ -2421,7 +2234,7 @@
   <dimension ref="A1:A501"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A493" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A514" sqref="A514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4940,259 +4753,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A48"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>548</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>